<commit_message>
Projeto completo, faltando etapa 5
</commit_message>
<xml_diff>
--- a/Calamidade.xlsx
+++ b/Calamidade.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdaa4e8704868404/Documentos/Cdados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdaa4e8704868404/Documentos/Cdados/projeto 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="601" documentId="11_4A969315AC9395E79A8696671FBAEB45E12C4660" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95F10C15-BE4B-4D51-A4DC-B14D33396DC1}"/>
+  <xr:revisionPtr revIDLastSave="777" documentId="11_4A969315AC9395E79A8696671FBAEB45E12C4660" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E353A05-10BA-46B4-A84D-F490FBB31BB6}"/>
   <bookViews>
-    <workbookView xWindow="-11730" yWindow="3130" windowWidth="17370" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="603">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2195,12 +2195,60 @@
   <si>
     <t>terminei o primeiro epsodio de calamidade e eu nunca assisti algo tão épico incrível perfeito maravilhoso em toda minha vida, acho q eu nasci pra ver isso, que equipe perfeita</t>
   </si>
+  <si>
+    <t>me disseram que sábado vamos ter uma visita italiana aqui 👀 #calamidade</t>
+  </si>
+  <si>
+    <t>estado de sítio é o escambau! estado de calamidade pública!!!
+#impeachmentbolsonarourgente https://t.co/si8otukeqx</t>
+  </si>
+  <si>
+    <t>"dilma rousseff deve renunciar já, para poupar o país do trauma do impeachment e superar tanto o impasse que o mantém atolado como a calamidade sem precedentes do atual governo."
+https://t.co/ogktxyriki https://t.co/eok5kge0pz</t>
+  </si>
+  <si>
+    <t>ib pro squad da calamidade</t>
+  </si>
+  <si>
+    <t>o hoteleiro avisou desde o início pra nunca abrir a porta pra criança perguntando se você é a mamãe dela. #calamidade</t>
+  </si>
+  <si>
+    <t>o mcc vai passar na msm hora q calamidade eu quwro pular</t>
+  </si>
+  <si>
+    <t>#calamidade 
+balu parece mais com um:</t>
+  </si>
+  <si>
+    <t>thiago / dante
+liz / carina
+daniel / joui osnf
+#calamidade https://t.co/nwjmn4hefw</t>
+  </si>
+  <si>
+    <t>@lynkd13 tá ligado que o queen é a melhor calamidade e se pa o melhor comandante de yonkou né</t>
+  </si>
+  <si>
+    <t>@linkzin125 link(diminutivo) eu tenho a teoria q talvez a outra metade de kian a parte do conhecimento seja uma relíquia da calamidade já que o kian queria virar um marcado para talvez usar essa relíquia de conhecimento</t>
+  </si>
+  <si>
+    <t>@efervicente encontrei! okay, não a enxerguei com olhos empáticos de fato. peço perdão! talvez uma possível sugestão seria regular a distribuição desses benefícios e certificar-se que estão sendo entregues a população que realmente precisa e que está em estado de calamidade. não à todos.</t>
+  </si>
+  <si>
+    <t>01h47 da madrugada, vim tomar um banho e sem querer encontrei a fita que prende o fio do microfone que faço live todo dia ainda nas minhas costas. nem meu marido pra avisar. tô em estado de abandono e calamidade, meu deus….. https://t.co/cglxi16q15</t>
+  </si>
+  <si>
+    <t>@celibvt uma vez vi um tweet assim "isso doi tanto" foto do arthur sorrindo em desconjuracao e uma foto dele sério em calamidade nao aguentei kkkkkkkkkkkkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>amanhã finalmente eu vou conseguir assistir calamidade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2210,6 +2258,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2252,11 +2308,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2595,10 +2653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B387"/>
+  <dimension ref="A1:C503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
+      <selection activeCell="A402" sqref="A402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5702,17 +5760,139 @@
         <v>1</v>
       </c>
     </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A388" t="s">
+        <v>589</v>
+      </c>
+      <c r="B388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A389" t="s">
+        <v>590</v>
+      </c>
+      <c r="B389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A390" t="s">
+        <v>591</v>
+      </c>
+      <c r="B390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A391" t="s">
+        <v>592</v>
+      </c>
+      <c r="B391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A392" t="s">
+        <v>593</v>
+      </c>
+      <c r="B392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A393" t="s">
+        <v>594</v>
+      </c>
+      <c r="B393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A394" t="s">
+        <v>595</v>
+      </c>
+      <c r="B394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A395" t="s">
+        <v>596</v>
+      </c>
+      <c r="B395">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A396" t="s">
+        <v>597</v>
+      </c>
+      <c r="B396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A397" t="s">
+        <v>598</v>
+      </c>
+      <c r="B397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A398" t="s">
+        <v>599</v>
+      </c>
+      <c r="B398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A399" t="s">
+        <v>600</v>
+      </c>
+      <c r="B399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A400" t="s">
+        <v>601</v>
+      </c>
+      <c r="B400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A401" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="B401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A490" s="2"/>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C492" s="2"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A503" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202:XFD207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5720,7 +5900,7 @@
     <col min="1" max="1" width="84.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
@@ -5728,19 +5908,15 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>302</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>SUM(B2:B501)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>303</v>
       </c>
@@ -5748,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -5756,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>305</v>
       </c>
@@ -5764,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>306</v>
       </c>
@@ -5772,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>307</v>
       </c>
@@ -5780,7 +5956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>308</v>
       </c>
@@ -5788,7 +5964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>309</v>
       </c>
@@ -5796,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>310</v>
       </c>
@@ -5804,7 +5980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>311</v>
       </c>
@@ -5812,7 +5988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>312</v>
       </c>
@@ -5820,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>313</v>
       </c>
@@ -5828,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>314</v>
       </c>
@@ -5836,7 +6012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>315</v>
       </c>
@@ -5844,7 +6020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>316</v>
       </c>
@@ -7334,5 +7510,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>